<commit_message>
binary done, rank with 12 workers, names drawn from excel
</commit_message>
<xml_diff>
--- a/_static/global/workers_binary_mat.xlsx
+++ b/_static/global/workers_binary_mat.xlsx
@@ -2442,9 +2442,6 @@
     <t>matrices</t>
   </si>
   <si>
-    <t>matrices_rank</t>
-  </si>
-  <si>
     <t>re_rank</t>
   </si>
   <si>
@@ -2452,6 +2449,9 @@
   </si>
   <si>
     <t>re_range</t>
+  </si>
+  <si>
+    <t>mat_rank</t>
   </si>
 </sst>
 </file>
@@ -2843,7 +2843,7 @@
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="CF1" sqref="CF1"/>
-      <selection pane="bottomLeft" activeCell="BU6" sqref="BU6"/>
+      <selection pane="bottomLeft" activeCell="BU1" sqref="BU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3137,16 +3137,16 @@
         <v>69</v>
       </c>
       <c r="BU1" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="BV1" s="7" t="s">
         <v>806</v>
       </c>
-      <c r="BV1" s="7" t="s">
+      <c r="BW1" s="7" t="s">
         <v>807</v>
       </c>
-      <c r="BW1" s="7" t="s">
+      <c r="BX1" s="7" t="s">
         <v>808</v>
-      </c>
-      <c r="BX1" s="7" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="2" spans="1:76" x14ac:dyDescent="0.35">
@@ -3360,19 +3360,19 @@
         <v>23</v>
       </c>
       <c r="BU2">
-        <f>_xlfn.RANK.EQ(BS2,$BS$2:$BS$97)</f>
+        <f t="shared" ref="BU2:BU33" si="2">_xlfn.RANK.EQ(BS2,$BS$2:$BS$97)</f>
         <v>1</v>
       </c>
       <c r="BV2">
-        <f>_xlfn.RANK.EQ(AI2,$AI$2:$AI$97)</f>
+        <f t="shared" ref="BV2:BV33" si="3">_xlfn.RANK.EQ(AI2,$AI$2:$AI$97)</f>
         <v>30</v>
       </c>
       <c r="BW2" t="str">
-        <f>IF(BU2&lt;=5,"Top 5",IF(BU2&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" ref="BW2:BX6" si="4">IF(BU2&lt;=5,"Top 5",IF(BU2&gt;=11,"Bottom 5","Middle 5"))</f>
         <v>Top 5</v>
       </c>
       <c r="BX2" t="str">
-        <f>IF(BV2&lt;=5,"Top 5",IF(BV2&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -3590,19 +3590,19 @@
         <v>20</v>
       </c>
       <c r="BU3">
-        <f>_xlfn.RANK.EQ(BS3,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="BV3">
-        <f>_xlfn.RANK.EQ(AI3,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="BW3" t="str">
-        <f>IF(BU3&lt;=5,"Top 5",IF(BU3&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Middle 5</v>
       </c>
       <c r="BX3" t="str">
-        <f>IF(BV3&lt;=5,"Top 5",IF(BV3&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -3817,19 +3817,19 @@
         <v>20.5</v>
       </c>
       <c r="BU4">
-        <f>_xlfn.RANK.EQ(BS4,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV4">
-        <f>_xlfn.RANK.EQ(AI4,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="BW4" t="str">
-        <f>IF(BU4&lt;=5,"Top 5",IF(BU4&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX4" t="str">
-        <f>IF(BV4&lt;=5,"Top 5",IF(BV4&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -4044,19 +4044,19 @@
         <v>15</v>
       </c>
       <c r="BU5">
-        <f>_xlfn.RANK.EQ(BS5,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="BV5">
-        <f>_xlfn.RANK.EQ(AI5,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="BW5" t="str">
-        <f>IF(BU5&lt;=5,"Top 5",IF(BU5&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Middle 5</v>
       </c>
       <c r="BX5" t="str">
-        <f>IF(BV5&lt;=5,"Top 5",IF(BV5&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -4277,19 +4277,19 @@
         <v>23.5</v>
       </c>
       <c r="BU6">
-        <f>_xlfn.RANK.EQ(BS6,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="BV6">
-        <f>_xlfn.RANK.EQ(AI6,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="BW6" t="str">
-        <f>IF(BU6&lt;=5,"Top 5",IF(BU6&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Top 5</v>
       </c>
       <c r="BX6" t="str">
-        <f>IF(BV6&lt;=5,"Top 5",IF(BV6&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" si="4"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -4504,19 +4504,19 @@
         <v>20.51</v>
       </c>
       <c r="BU7">
-        <f>_xlfn.RANK.EQ(BS7,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="BV7">
-        <f>_xlfn.RANK.EQ(AI7,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="BW7" t="str">
-        <f t="shared" ref="BW7:BW66" si="2">IF(BU7&lt;=5,"Top 5",IF(BU7&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" ref="BW7:BW66" si="5">IF(BU7&lt;=5,"Top 5",IF(BU7&gt;=11,"Bottom 5","Middle 5"))</f>
         <v>Top 5</v>
       </c>
       <c r="BX7" t="str">
-        <f t="shared" ref="BX7:BX66" si="3">IF(BV7&lt;=5,"Top 5",IF(BV7&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" ref="BX7:BX66" si="6">IF(BV7&lt;=5,"Top 5",IF(BV7&gt;=11,"Bottom 5","Middle 5"))</f>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -4731,19 +4731,19 @@
         <v>18</v>
       </c>
       <c r="BU8">
-        <f>_xlfn.RANK.EQ(BS8,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="BV8">
-        <f>_xlfn.RANK.EQ(AI8,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="BW8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Top 5</v>
       </c>
       <c r="BX8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -4949,19 +4949,19 @@
         <v>26.4</v>
       </c>
       <c r="BU9">
-        <f>_xlfn.RANK.EQ(BS9,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="BV9">
-        <f>_xlfn.RANK.EQ(AI9,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="BW9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Top 5</v>
       </c>
       <c r="BX9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Top 5</v>
       </c>
     </row>
@@ -5179,19 +5179,19 @@
         <v>21.5</v>
       </c>
       <c r="BU10">
-        <f>_xlfn.RANK.EQ(BS10,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="BV10">
-        <f>_xlfn.RANK.EQ(AI10,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="BW10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Top 5</v>
       </c>
       <c r="BX10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -5403,19 +5403,19 @@
         <v>21</v>
       </c>
       <c r="BU11">
-        <f>_xlfn.RANK.EQ(BS11,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="BV11">
-        <f>_xlfn.RANK.EQ(AI11,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="BW11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Top 5</v>
       </c>
       <c r="BX11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -5636,19 +5636,19 @@
         <v>19.5</v>
       </c>
       <c r="BU12">
-        <f>_xlfn.RANK.EQ(BS12,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="BV12">
-        <f>_xlfn.RANK.EQ(AI12,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="BW12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Top 5</v>
       </c>
       <c r="BX12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -5869,19 +5869,19 @@
         <v>19</v>
       </c>
       <c r="BU13">
-        <f>_xlfn.RANK.EQ(BS13,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="BV13">
-        <f>_xlfn.RANK.EQ(AI13,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="BW13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Top 5</v>
       </c>
       <c r="BX13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -6087,19 +6087,19 @@
         <v>22</v>
       </c>
       <c r="BU14">
-        <f>_xlfn.RANK.EQ(BS14,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="BV14">
-        <f>_xlfn.RANK.EQ(AI14,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="BW14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Middle 5</v>
       </c>
       <c r="BX14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -6317,19 +6317,19 @@
         <v>12</v>
       </c>
       <c r="BU15">
-        <f>_xlfn.RANK.EQ(BS15,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="BV15">
-        <f>_xlfn.RANK.EQ(AI15,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="BW15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Middle 5</v>
       </c>
       <c r="BX15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -6547,19 +6547,19 @@
         <v>23</v>
       </c>
       <c r="BU16">
-        <f>_xlfn.RANK.EQ(BS16,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV16">
-        <f>_xlfn.RANK.EQ(AI16,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="BW16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Top 5</v>
       </c>
     </row>
@@ -6771,19 +6771,19 @@
         <v>21.5</v>
       </c>
       <c r="BU17">
-        <f>_xlfn.RANK.EQ(BS17,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV17">
-        <f>_xlfn.RANK.EQ(AI17,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="BW17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -7001,19 +7001,19 @@
         <v>19.489999999999998</v>
       </c>
       <c r="BU18">
-        <f>_xlfn.RANK.EQ(BS18,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV18">
-        <f>_xlfn.RANK.EQ(AI18,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="BW18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -7225,19 +7225,19 @@
         <v>14</v>
       </c>
       <c r="BU19">
-        <f>_xlfn.RANK.EQ(BS19,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV19">
-        <f>_xlfn.RANK.EQ(AI19,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="BW19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -7458,19 +7458,19 @@
         <v>13.5</v>
       </c>
       <c r="BU20">
-        <f>_xlfn.RANK.EQ(BS20,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV20">
-        <f>_xlfn.RANK.EQ(AI20,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="BW20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -7685,19 +7685,19 @@
         <v>13</v>
       </c>
       <c r="BU21">
-        <f>_xlfn.RANK.EQ(BS21,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="BV21">
-        <f>_xlfn.RANK.EQ(AI21,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="BW21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -7915,19 +7915,19 @@
         <v>25</v>
       </c>
       <c r="BU22">
-        <f>_xlfn.RANK.EQ(BS22,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV22">
-        <f>_xlfn.RANK.EQ(AI22,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="BW22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Top 5</v>
       </c>
     </row>
@@ -8139,19 +8139,19 @@
         <v>23</v>
       </c>
       <c r="BU23">
-        <f>_xlfn.RANK.EQ(BS23,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV23">
-        <f>_xlfn.RANK.EQ(AI23,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="BW23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -8357,19 +8357,19 @@
         <v>20.5</v>
       </c>
       <c r="BU24">
-        <f>_xlfn.RANK.EQ(BS24,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV24">
-        <f>_xlfn.RANK.EQ(AI24,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="BW24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -8581,19 +8581,19 @@
         <v>19.5</v>
       </c>
       <c r="BU25">
-        <f>_xlfn.RANK.EQ(BS25,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV25">
-        <f>_xlfn.RANK.EQ(AI25,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="BW25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -8811,19 +8811,19 @@
         <v>18.2</v>
       </c>
       <c r="BU26">
-        <f>_xlfn.RANK.EQ(BS26,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV26">
-        <f>_xlfn.RANK.EQ(AI26,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="BW26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -9038,19 +9038,19 @@
         <v>17.68</v>
       </c>
       <c r="BU27">
-        <f>_xlfn.RANK.EQ(BS27,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV27">
-        <f>_xlfn.RANK.EQ(AI27,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="BW27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -9265,19 +9265,19 @@
         <v>17</v>
       </c>
       <c r="BU28">
-        <f>_xlfn.RANK.EQ(BS28,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV28">
-        <f>_xlfn.RANK.EQ(AI28,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="BW28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -9495,19 +9495,19 @@
         <v>14.5</v>
       </c>
       <c r="BU29">
-        <f>_xlfn.RANK.EQ(BS29,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV29">
-        <f>_xlfn.RANK.EQ(AI29,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="BW29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -9722,19 +9722,19 @@
         <v>14</v>
       </c>
       <c r="BU30">
-        <f>_xlfn.RANK.EQ(BS30,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV30">
-        <f>_xlfn.RANK.EQ(AI30,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="BW30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -9943,19 +9943,19 @@
         <v>11</v>
       </c>
       <c r="BU31">
-        <f>_xlfn.RANK.EQ(BS31,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="BV31">
-        <f>_xlfn.RANK.EQ(AI31,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="BW31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -10170,19 +10170,19 @@
         <v>20</v>
       </c>
       <c r="BU32">
-        <f>_xlfn.RANK.EQ(BS32,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="BV32">
-        <f>_xlfn.RANK.EQ(AI32,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="BW32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -10397,19 +10397,19 @@
         <v>18</v>
       </c>
       <c r="BU33">
-        <f>_xlfn.RANK.EQ(BS33,$BS$2:$BS$97)</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="BV33">
-        <f>_xlfn.RANK.EQ(AI33,$AI$2:$AI$97)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="BW33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -10601,27 +10601,27 @@
         <v>10</v>
       </c>
       <c r="BS34">
-        <f t="shared" ref="BS34:BS65" si="4">AE34+AF34+AG34</f>
+        <f t="shared" ref="BS34:BS65" si="7">AE34+AF34+AG34</f>
         <v>9</v>
       </c>
       <c r="BT34">
-        <f t="shared" ref="BT34:BT65" si="5">BS34+AI34+AH34</f>
+        <f t="shared" ref="BT34:BT65" si="8">BS34+AI34+AH34</f>
         <v>18</v>
       </c>
       <c r="BU34">
-        <f>_xlfn.RANK.EQ(BS34,$BS$2:$BS$97)</f>
+        <f t="shared" ref="BU34:BU65" si="9">_xlfn.RANK.EQ(BS34,$BS$2:$BS$97)</f>
         <v>31</v>
       </c>
       <c r="BV34">
-        <f>_xlfn.RANK.EQ(AI34,$AI$2:$AI$97)</f>
+        <f t="shared" ref="BV34:BV65" si="10">_xlfn.RANK.EQ(AI34,$AI$2:$AI$97)</f>
         <v>18</v>
       </c>
       <c r="BW34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -10831,27 +10831,27 @@
         <v>5</v>
       </c>
       <c r="BS35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="BT35">
+        <f t="shared" si="8"/>
+        <v>15.69</v>
+      </c>
+      <c r="BU35">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="BV35">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BW35" t="str">
         <f t="shared" si="5"/>
-        <v>15.69</v>
-      </c>
-      <c r="BU35">
-        <f>_xlfn.RANK.EQ(BS35,$BS$2:$BS$97)</f>
-        <v>31</v>
-      </c>
-      <c r="BV35">
-        <f>_xlfn.RANK.EQ(AI35,$AI$2:$AI$97)</f>
-        <v>48</v>
-      </c>
-      <c r="BW35" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
       <c r="BY35"/>
@@ -11063,27 +11063,27 @@
         <v>11</v>
       </c>
       <c r="BS36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="BT36">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+      <c r="BU36">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="BV36">
+        <f t="shared" si="10"/>
+        <v>59</v>
+      </c>
+      <c r="BW36" t="str">
         <f t="shared" si="5"/>
-        <v>14.5</v>
-      </c>
-      <c r="BU36">
-        <f>_xlfn.RANK.EQ(BS36,$BS$2:$BS$97)</f>
-        <v>31</v>
-      </c>
-      <c r="BV36">
-        <f>_xlfn.RANK.EQ(AI36,$AI$2:$AI$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BW36" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -11293,27 +11293,27 @@
         <v>6</v>
       </c>
       <c r="BS37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="BT37">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="BU37">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="BV37">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BW37" t="str">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="BU37">
-        <f>_xlfn.RANK.EQ(BS37,$BS$2:$BS$97)</f>
-        <v>31</v>
-      </c>
-      <c r="BV37">
-        <f>_xlfn.RANK.EQ(AI37,$AI$2:$AI$97)</f>
-        <v>48</v>
-      </c>
-      <c r="BW37" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -11520,27 +11520,27 @@
         <v>8</v>
       </c>
       <c r="BS38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="BT38">
+        <f t="shared" si="8"/>
+        <v>13.5</v>
+      </c>
+      <c r="BU38">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="BV38">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="BW38" t="str">
         <f t="shared" si="5"/>
-        <v>13.5</v>
-      </c>
-      <c r="BU38">
-        <f>_xlfn.RANK.EQ(BS38,$BS$2:$BS$97)</f>
-        <v>31</v>
-      </c>
-      <c r="BV38">
-        <f>_xlfn.RANK.EQ(AI38,$AI$2:$AI$97)</f>
-        <v>64</v>
-      </c>
-      <c r="BW38" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -11750,27 +11750,27 @@
         <v>13</v>
       </c>
       <c r="BS39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT39">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="BU39">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV39">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="BW39" t="str">
         <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="BU39">
-        <f>_xlfn.RANK.EQ(BS39,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV39">
-        <f>_xlfn.RANK.EQ(AI39,$AI$2:$AI$97)</f>
-        <v>8</v>
-      </c>
-      <c r="BW39" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
       <c r="BY39" s="3"/>
@@ -11988,27 +11988,27 @@
         <v>11</v>
       </c>
       <c r="BS40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT40">
+        <f t="shared" si="8"/>
+        <v>21.5</v>
+      </c>
+      <c r="BU40">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV40">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="BW40" t="str">
         <f t="shared" si="5"/>
-        <v>21.5</v>
-      </c>
-      <c r="BU40">
-        <f>_xlfn.RANK.EQ(BS40,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV40">
-        <f>_xlfn.RANK.EQ(AI40,$AI$2:$AI$97)</f>
-        <v>4</v>
-      </c>
-      <c r="BW40" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Top 5</v>
       </c>
     </row>
@@ -12215,27 +12215,27 @@
         <v>9</v>
       </c>
       <c r="BS41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT41">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="BU41">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV41">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="BW41" t="str">
         <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="BU41">
-        <f>_xlfn.RANK.EQ(BS41,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV41">
-        <f>_xlfn.RANK.EQ(AI41,$AI$2:$AI$97)</f>
-        <v>10</v>
-      </c>
-      <c r="BW41" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -12436,27 +12436,27 @@
         <v>7</v>
       </c>
       <c r="BS42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT42">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="BU42">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV42">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="BW42" t="str">
         <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="BU42">
-        <f>_xlfn.RANK.EQ(BS42,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV42">
-        <f>_xlfn.RANK.EQ(AI42,$AI$2:$AI$97)</f>
-        <v>18</v>
-      </c>
-      <c r="BW42" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -12666,27 +12666,27 @@
         <v>7</v>
       </c>
       <c r="BS43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT43">
+        <f t="shared" si="8"/>
+        <v>15.9</v>
+      </c>
+      <c r="BU43">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV43">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="BW43" t="str">
         <f t="shared" si="5"/>
-        <v>15.9</v>
-      </c>
-      <c r="BU43">
-        <f>_xlfn.RANK.EQ(BS43,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV43">
-        <f>_xlfn.RANK.EQ(AI43,$AI$2:$AI$97)</f>
-        <v>30</v>
-      </c>
-      <c r="BW43" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -12898,27 +12898,27 @@
         <v>14</v>
       </c>
       <c r="BS44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT44">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+      <c r="BU44">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV44">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BW44" t="str">
         <f t="shared" si="5"/>
-        <v>14.5</v>
-      </c>
-      <c r="BU44">
-        <f>_xlfn.RANK.EQ(BS44,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV44">
-        <f>_xlfn.RANK.EQ(AI44,$AI$2:$AI$97)</f>
-        <v>48</v>
-      </c>
-      <c r="BW44" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -13125,27 +13125,27 @@
         <v>7.98</v>
       </c>
       <c r="BS45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT45">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="BU45">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV45">
+        <f t="shared" si="10"/>
+        <v>39</v>
+      </c>
+      <c r="BW45" t="str">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="BU45">
-        <f>_xlfn.RANK.EQ(BS45,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV45">
-        <f>_xlfn.RANK.EQ(AI45,$AI$2:$AI$97)</f>
-        <v>39</v>
-      </c>
-      <c r="BW45" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -13346,27 +13346,27 @@
         <v>15</v>
       </c>
       <c r="BS46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT46">
+        <f t="shared" si="8"/>
+        <v>12.52</v>
+      </c>
+      <c r="BU46">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV46">
+        <f t="shared" si="10"/>
+        <v>85</v>
+      </c>
+      <c r="BW46" t="str">
         <f t="shared" si="5"/>
-        <v>12.52</v>
-      </c>
-      <c r="BU46">
-        <f>_xlfn.RANK.EQ(BS46,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV46">
-        <f>_xlfn.RANK.EQ(AI46,$AI$2:$AI$97)</f>
-        <v>85</v>
-      </c>
-      <c r="BW46" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -13570,27 +13570,27 @@
         <v>10</v>
       </c>
       <c r="BS47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT47">
+        <f t="shared" si="8"/>
+        <v>11.27</v>
+      </c>
+      <c r="BU47">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV47">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="BW47" t="str">
         <f t="shared" si="5"/>
-        <v>11.27</v>
-      </c>
-      <c r="BU47">
-        <f>_xlfn.RANK.EQ(BS47,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV47">
-        <f>_xlfn.RANK.EQ(AI47,$AI$2:$AI$97)</f>
-        <v>64</v>
-      </c>
-      <c r="BW47" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -13797,27 +13797,27 @@
         <v>9</v>
       </c>
       <c r="BS48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT48">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="BU48">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV48">
+        <f t="shared" si="10"/>
+        <v>76</v>
+      </c>
+      <c r="BW48" t="str">
         <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="BU48">
-        <f>_xlfn.RANK.EQ(BS48,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV48">
-        <f>_xlfn.RANK.EQ(AI48,$AI$2:$AI$97)</f>
-        <v>76</v>
-      </c>
-      <c r="BW48" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -14018,27 +14018,27 @@
         <v>8</v>
       </c>
       <c r="BS49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT49">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="BU49">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV49">
+        <f t="shared" si="10"/>
+        <v>76</v>
+      </c>
+      <c r="BW49" t="str">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="BU49">
-        <f>_xlfn.RANK.EQ(BS49,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV49">
-        <f>_xlfn.RANK.EQ(AI49,$AI$2:$AI$97)</f>
-        <v>76</v>
-      </c>
-      <c r="BW49" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -14239,27 +14239,27 @@
         <v>2</v>
       </c>
       <c r="BS50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="BT50">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="BU50">
+        <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="BV50">
+        <f t="shared" si="10"/>
+        <v>76</v>
+      </c>
+      <c r="BW50" t="str">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="BU50">
-        <f>_xlfn.RANK.EQ(BS50,$BS$2:$BS$97)</f>
-        <v>38</v>
-      </c>
-      <c r="BV50">
-        <f>_xlfn.RANK.EQ(AI50,$AI$2:$AI$97)</f>
-        <v>76</v>
-      </c>
-      <c r="BW50" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -14463,27 +14463,27 @@
         <v>10</v>
       </c>
       <c r="BS51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="BT51">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="BU51">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="BV51">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="BW51" t="str">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="BU51">
-        <f>_xlfn.RANK.EQ(BS51,$BS$2:$BS$97)</f>
-        <v>50</v>
-      </c>
-      <c r="BV51">
-        <f>_xlfn.RANK.EQ(AI51,$AI$2:$AI$97)</f>
-        <v>30</v>
-      </c>
-      <c r="BW51" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -14681,27 +14681,27 @@
         <v>16</v>
       </c>
       <c r="BS52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="BT52">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="BU52">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="BV52">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="BW52" t="str">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="BU52">
-        <f>_xlfn.RANK.EQ(BS52,$BS$2:$BS$97)</f>
-        <v>50</v>
-      </c>
-      <c r="BV52">
-        <f>_xlfn.RANK.EQ(AI52,$AI$2:$AI$97)</f>
-        <v>4</v>
-      </c>
-      <c r="BW52" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Top 5</v>
       </c>
     </row>
@@ -14899,27 +14899,27 @@
         <v>8</v>
       </c>
       <c r="BS53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="BT53">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+      <c r="BU53">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="BV53">
+        <f t="shared" si="10"/>
+        <v>39</v>
+      </c>
+      <c r="BW53" t="str">
         <f t="shared" si="5"/>
-        <v>14.5</v>
-      </c>
-      <c r="BU53">
-        <f>_xlfn.RANK.EQ(BS53,$BS$2:$BS$97)</f>
-        <v>50</v>
-      </c>
-      <c r="BV53">
-        <f>_xlfn.RANK.EQ(AI53,$AI$2:$AI$97)</f>
-        <v>39</v>
-      </c>
-      <c r="BW53" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -15129,27 +15129,27 @@
         <v>12</v>
       </c>
       <c r="BS54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="BT54">
+        <f t="shared" si="8"/>
+        <v>13.48</v>
+      </c>
+      <c r="BU54">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="BV54">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="BW54" t="str">
         <f t="shared" si="5"/>
-        <v>13.48</v>
-      </c>
-      <c r="BU54">
-        <f>_xlfn.RANK.EQ(BS54,$BS$2:$BS$97)</f>
-        <v>53</v>
-      </c>
-      <c r="BV54">
-        <f>_xlfn.RANK.EQ(AI54,$AI$2:$AI$97)</f>
-        <v>18</v>
-      </c>
-      <c r="BW54" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
       <c r="BY54" s="3"/>
@@ -15367,27 +15367,27 @@
         <v>7</v>
       </c>
       <c r="BS55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="BT55">
+        <f t="shared" si="8"/>
+        <v>12.5</v>
+      </c>
+      <c r="BU55">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="BV55">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BW55" t="str">
         <f t="shared" si="5"/>
-        <v>12.5</v>
-      </c>
-      <c r="BU55">
-        <f>_xlfn.RANK.EQ(BS55,$BS$2:$BS$97)</f>
-        <v>53</v>
-      </c>
-      <c r="BV55">
-        <f>_xlfn.RANK.EQ(AI55,$AI$2:$AI$97)</f>
-        <v>48</v>
-      </c>
-      <c r="BW55" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -15594,27 +15594,27 @@
         <v>7</v>
       </c>
       <c r="BS56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="BT56">
+        <f t="shared" si="8"/>
+        <v>12.02</v>
+      </c>
+      <c r="BU56">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="BV56">
+        <f t="shared" si="10"/>
+        <v>39</v>
+      </c>
+      <c r="BW56" t="str">
         <f t="shared" si="5"/>
-        <v>12.02</v>
-      </c>
-      <c r="BU56">
-        <f>_xlfn.RANK.EQ(BS56,$BS$2:$BS$97)</f>
-        <v>53</v>
-      </c>
-      <c r="BV56">
-        <f>_xlfn.RANK.EQ(AI56,$AI$2:$AI$97)</f>
-        <v>39</v>
-      </c>
-      <c r="BW56" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -15728,27 +15728,27 @@
         <v>15</v>
       </c>
       <c r="BS57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="BT57">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="BU57">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="BV57">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="BW57" t="str">
         <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="BU57">
-        <f>_xlfn.RANK.EQ(BS57,$BS$2:$BS$97)</f>
-        <v>53</v>
-      </c>
-      <c r="BV57">
-        <f>_xlfn.RANK.EQ(AI57,$AI$2:$AI$97)</f>
-        <v>64</v>
-      </c>
-      <c r="BW57" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -15952,27 +15952,27 @@
         <v>9</v>
       </c>
       <c r="BS58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="BT58">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="BU58">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="BV58">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BW58" t="str">
         <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="BU58">
-        <f>_xlfn.RANK.EQ(BS58,$BS$2:$BS$97)</f>
-        <v>53</v>
-      </c>
-      <c r="BV58">
-        <f>_xlfn.RANK.EQ(AI58,$AI$2:$AI$97)</f>
-        <v>48</v>
-      </c>
-      <c r="BW58" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -16182,27 +16182,27 @@
         <v>15</v>
       </c>
       <c r="BS59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="BT59">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="BU59">
+        <f t="shared" si="9"/>
+        <v>53</v>
+      </c>
+      <c r="BV59">
+        <f t="shared" si="10"/>
+        <v>64</v>
+      </c>
+      <c r="BW59" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="BU59">
-        <f>_xlfn.RANK.EQ(BS59,$BS$2:$BS$97)</f>
-        <v>53</v>
-      </c>
-      <c r="BV59">
-        <f>_xlfn.RANK.EQ(AI59,$AI$2:$AI$97)</f>
-        <v>64</v>
-      </c>
-      <c r="BW59" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -16409,27 +16409,27 @@
         <v>13</v>
       </c>
       <c r="BS60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT60">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="BU60">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="BV60">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="BW60" t="str">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="BU60">
-        <f>_xlfn.RANK.EQ(BS60,$BS$2:$BS$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BV60">
-        <f>_xlfn.RANK.EQ(AI60,$AI$2:$AI$97)</f>
-        <v>10</v>
-      </c>
-      <c r="BW60" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Middle 5</v>
       </c>
     </row>
@@ -16639,27 +16639,27 @@
         <v>5</v>
       </c>
       <c r="BS61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT61">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+      <c r="BU61">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="BV61">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="BW61" t="str">
         <f t="shared" si="5"/>
-        <v>14.5</v>
-      </c>
-      <c r="BU61">
-        <f>_xlfn.RANK.EQ(BS61,$BS$2:$BS$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BV61">
-        <f>_xlfn.RANK.EQ(AI61,$AI$2:$AI$97)</f>
-        <v>18</v>
-      </c>
-      <c r="BW61" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -16866,27 +16866,27 @@
         <v>3</v>
       </c>
       <c r="BS62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT62">
+        <f t="shared" si="8"/>
+        <v>14.5</v>
+      </c>
+      <c r="BU62">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="BV62">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="BW62" t="str">
         <f t="shared" si="5"/>
-        <v>14.5</v>
-      </c>
-      <c r="BU62">
-        <f>_xlfn.RANK.EQ(BS62,$BS$2:$BS$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BV62">
-        <f>_xlfn.RANK.EQ(AI62,$AI$2:$AI$97)</f>
-        <v>18</v>
-      </c>
-      <c r="BW62" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -17090,27 +17090,27 @@
         <v>13</v>
       </c>
       <c r="BS63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT63">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="BU63">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="BV63">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="BW63" t="str">
         <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="BU63">
-        <f>_xlfn.RANK.EQ(BS63,$BS$2:$BS$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BV63">
-        <f>_xlfn.RANK.EQ(AI63,$AI$2:$AI$97)</f>
-        <v>30</v>
-      </c>
-      <c r="BW63" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -17308,27 +17308,27 @@
         <v>0.99</v>
       </c>
       <c r="BS64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT64">
+        <f t="shared" si="8"/>
+        <v>12.35</v>
+      </c>
+      <c r="BU64">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="BV64">
+        <f t="shared" si="10"/>
+        <v>39</v>
+      </c>
+      <c r="BW64" t="str">
         <f t="shared" si="5"/>
-        <v>12.35</v>
-      </c>
-      <c r="BU64">
-        <f>_xlfn.RANK.EQ(BS64,$BS$2:$BS$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BV64">
-        <f>_xlfn.RANK.EQ(AI64,$AI$2:$AI$97)</f>
-        <v>39</v>
-      </c>
-      <c r="BW64" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -17535,27 +17535,27 @@
         <v>8</v>
       </c>
       <c r="BS65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="BT65">
+        <f t="shared" si="8"/>
+        <v>10.52</v>
+      </c>
+      <c r="BU65">
+        <f t="shared" si="9"/>
+        <v>59</v>
+      </c>
+      <c r="BV65">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="BW65" t="str">
         <f t="shared" si="5"/>
-        <v>10.52</v>
-      </c>
-      <c r="BU65">
-        <f>_xlfn.RANK.EQ(BS65,$BS$2:$BS$97)</f>
-        <v>59</v>
-      </c>
-      <c r="BV65">
-        <f>_xlfn.RANK.EQ(AI65,$AI$2:$AI$97)</f>
-        <v>48</v>
-      </c>
-      <c r="BW65" t="str">
-        <f t="shared" si="2"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -17765,27 +17765,27 @@
         <v>9</v>
       </c>
       <c r="BS66">
-        <f t="shared" ref="BS66:BS97" si="6">AE66+AF66+AG66</f>
+        <f t="shared" ref="BS66:BS97" si="11">AE66+AF66+AG66</f>
         <v>5</v>
       </c>
       <c r="BT66">
-        <f t="shared" ref="BT66:BT97" si="7">BS66+AI66+AH66</f>
+        <f t="shared" ref="BT66:BT97" si="12">BS66+AI66+AH66</f>
         <v>10</v>
       </c>
       <c r="BU66">
-        <f>_xlfn.RANK.EQ(BS66,$BS$2:$BS$97)</f>
+        <f t="shared" ref="BU66:BU97" si="13">_xlfn.RANK.EQ(BS66,$BS$2:$BS$97)</f>
         <v>59</v>
       </c>
       <c r="BV66">
-        <f>_xlfn.RANK.EQ(AI66,$AI$2:$AI$97)</f>
+        <f t="shared" ref="BV66:BV97" si="14">_xlfn.RANK.EQ(AI66,$AI$2:$AI$97)</f>
         <v>85</v>
       </c>
       <c r="BW66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -17992,27 +17992,27 @@
         <v>14</v>
       </c>
       <c r="BS67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="BT67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="BU67">
-        <f>_xlfn.RANK.EQ(BS67,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="BV67">
-        <f>_xlfn.RANK.EQ(AI67,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="BW67" t="str">
-        <f t="shared" ref="BW67:BW97" si="8">IF(BU67&lt;=5,"Top 5",IF(BU67&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" ref="BW67:BW97" si="15">IF(BU67&lt;=5,"Top 5",IF(BU67&gt;=11,"Bottom 5","Middle 5"))</f>
         <v>Bottom 5</v>
       </c>
       <c r="BX67" t="str">
-        <f t="shared" ref="BX67:BX97" si="9">IF(BV67&lt;=5,"Top 5",IF(BV67&gt;=11,"Bottom 5","Middle 5"))</f>
+        <f t="shared" ref="BX67:BX97" si="16">IF(BV67&lt;=5,"Top 5",IF(BV67&gt;=11,"Bottom 5","Middle 5"))</f>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -18219,27 +18219,27 @@
         <v>9</v>
       </c>
       <c r="BS68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="BT68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>8.5</v>
       </c>
       <c r="BU68">
-        <f>_xlfn.RANK.EQ(BS68,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="BV68">
-        <f>_xlfn.RANK.EQ(AI68,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX68" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -18446,27 +18446,27 @@
         <v>8</v>
       </c>
       <c r="BS69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="BT69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.82</v>
       </c>
       <c r="BU69">
-        <f>_xlfn.RANK.EQ(BS69,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="BV69">
-        <f>_xlfn.RANK.EQ(AI69,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="BW69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX69" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -18676,27 +18676,27 @@
         <v>1</v>
       </c>
       <c r="BS70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="BT70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="BU70">
-        <f>_xlfn.RANK.EQ(BS70,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="BV70">
-        <f>_xlfn.RANK.EQ(AI70,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
       <c r="BY70"/>
@@ -18914,27 +18914,27 @@
         <v>6</v>
       </c>
       <c r="BS71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="BT71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="BU71">
-        <f>_xlfn.RANK.EQ(BS71,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="BV71">
-        <f>_xlfn.RANK.EQ(AI71,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX71" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -19132,27 +19132,27 @@
         <v>2</v>
       </c>
       <c r="BS72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="BT72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="BU72">
-        <f>_xlfn.RANK.EQ(BS72,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="BV72">
-        <f>_xlfn.RANK.EQ(AI72,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -19359,27 +19359,27 @@
         <v>9</v>
       </c>
       <c r="BS73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>11.5</v>
       </c>
       <c r="BU73">
-        <f>_xlfn.RANK.EQ(BS73,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV73">
-        <f>_xlfn.RANK.EQ(AI73,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>39</v>
       </c>
       <c r="BW73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX73" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -19586,27 +19586,27 @@
         <v>8</v>
       </c>
       <c r="BS74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>10.5</v>
       </c>
       <c r="BU74">
-        <f>_xlfn.RANK.EQ(BS74,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV74">
-        <f>_xlfn.RANK.EQ(AI74,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>48</v>
       </c>
       <c r="BW74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX74" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -19810,27 +19810,27 @@
         <v>14</v>
       </c>
       <c r="BS75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>9.4</v>
       </c>
       <c r="BU75">
-        <f>_xlfn.RANK.EQ(BS75,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV75">
-        <f>_xlfn.RANK.EQ(AI75,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="BW75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX75" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -20028,27 +20028,27 @@
         <v>10</v>
       </c>
       <c r="BS76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>8.35</v>
       </c>
       <c r="BU76">
-        <f>_xlfn.RANK.EQ(BS76,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV76">
-        <f>_xlfn.RANK.EQ(AI76,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="BW76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX76" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -20255,27 +20255,27 @@
         <v>14</v>
       </c>
       <c r="BS77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.03</v>
       </c>
       <c r="BU77">
-        <f>_xlfn.RANK.EQ(BS77,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV77">
-        <f>_xlfn.RANK.EQ(AI77,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="BW77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -20476,27 +20476,27 @@
         <v>10</v>
       </c>
       <c r="BS78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="BU78">
-        <f>_xlfn.RANK.EQ(BS78,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV78">
-        <f>_xlfn.RANK.EQ(AI78,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="BW78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX78" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -20703,27 +20703,27 @@
         <v>0.05</v>
       </c>
       <c r="BS79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5.4</v>
       </c>
       <c r="BU79">
-        <f>_xlfn.RANK.EQ(BS79,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV79">
-        <f>_xlfn.RANK.EQ(AI79,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="BW79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX79" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -20930,27 +20930,27 @@
         <v>12</v>
       </c>
       <c r="BS80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="BU80">
-        <f>_xlfn.RANK.EQ(BS80,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV80">
-        <f>_xlfn.RANK.EQ(AI80,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="BW80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX80" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -21157,27 +21157,27 @@
         <v>3</v>
       </c>
       <c r="BS81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="BT81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="BU81">
-        <f>_xlfn.RANK.EQ(BS81,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>72</v>
       </c>
       <c r="BV81">
-        <f>_xlfn.RANK.EQ(AI81,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX81" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -21372,27 +21372,27 @@
         <v>19</v>
       </c>
       <c r="BS82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>19</v>
       </c>
       <c r="BU82">
-        <f>_xlfn.RANK.EQ(BS82,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV82">
-        <f>_xlfn.RANK.EQ(AI82,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BW82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Top 5</v>
       </c>
     </row>
@@ -21593,27 +21593,27 @@
         <v>9</v>
       </c>
       <c r="BS83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="BU83">
-        <f>_xlfn.RANK.EQ(BS83,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV83">
-        <f>_xlfn.RANK.EQ(AI83,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="BW83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX83" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -21823,27 +21823,27 @@
         <v>15</v>
       </c>
       <c r="BS84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="BU84">
-        <f>_xlfn.RANK.EQ(BS84,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV84">
-        <f>_xlfn.RANK.EQ(AI84,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="BW84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX84" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -22056,27 +22056,27 @@
         <v>11</v>
       </c>
       <c r="BS85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="BU85">
-        <f>_xlfn.RANK.EQ(BS85,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV85">
-        <f>_xlfn.RANK.EQ(AI85,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>39</v>
       </c>
       <c r="BW85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX85" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -22280,27 +22280,27 @@
         <v>14</v>
       </c>
       <c r="BS86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>7.5</v>
       </c>
       <c r="BU86">
-        <f>_xlfn.RANK.EQ(BS86,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV86">
-        <f>_xlfn.RANK.EQ(AI86,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="BW86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX86" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -22510,27 +22510,27 @@
         <v>10</v>
       </c>
       <c r="BS87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.14</v>
       </c>
       <c r="BU87">
-        <f>_xlfn.RANK.EQ(BS87,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV87">
-        <f>_xlfn.RANK.EQ(AI87,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>59</v>
       </c>
       <c r="BW87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX87" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -22737,27 +22737,27 @@
         <v>12</v>
       </c>
       <c r="BS88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.01</v>
       </c>
       <c r="BU88">
-        <f>_xlfn.RANK.EQ(BS88,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV88">
-        <f>_xlfn.RANK.EQ(AI88,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW88" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX88" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -22961,27 +22961,27 @@
         <v>13</v>
       </c>
       <c r="BS89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.01</v>
       </c>
       <c r="BU89">
-        <f>_xlfn.RANK.EQ(BS89,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV89">
-        <f>_xlfn.RANK.EQ(AI89,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>76</v>
       </c>
       <c r="BW89" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX89" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -23188,27 +23188,27 @@
         <v>7</v>
       </c>
       <c r="BS90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="BT90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3.08</v>
       </c>
       <c r="BU90">
-        <f>_xlfn.RANK.EQ(BS90,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>81</v>
       </c>
       <c r="BV90">
-        <f>_xlfn.RANK.EQ(AI90,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW90" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX90" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -23415,27 +23415,27 @@
         <v>13.75</v>
       </c>
       <c r="BS91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="BT91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="BU91">
-        <f>_xlfn.RANK.EQ(BS91,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>90</v>
       </c>
       <c r="BV91">
-        <f>_xlfn.RANK.EQ(AI91,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="BW91" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX91" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -23639,27 +23639,27 @@
         <v>9</v>
       </c>
       <c r="BS92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="BT92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="BU92">
-        <f>_xlfn.RANK.EQ(BS92,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>90</v>
       </c>
       <c r="BV92">
-        <f>_xlfn.RANK.EQ(AI92,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="BW92" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX92" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -23857,27 +23857,27 @@
         <v>13</v>
       </c>
       <c r="BS93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="BT93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.5</v>
       </c>
       <c r="BU93">
-        <f>_xlfn.RANK.EQ(BS93,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>90</v>
       </c>
       <c r="BV93">
-        <f>_xlfn.RANK.EQ(AI93,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>85</v>
       </c>
       <c r="BW93" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX93" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -24087,27 +24087,27 @@
         <v>4</v>
       </c>
       <c r="BS94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="BT94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>10.55</v>
       </c>
       <c r="BU94">
-        <f>_xlfn.RANK.EQ(BS94,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>93</v>
       </c>
       <c r="BV94">
-        <f>_xlfn.RANK.EQ(AI94,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
       <c r="BW94" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX94" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -24308,27 +24308,27 @@
         <v>13</v>
       </c>
       <c r="BS95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="BT95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>9.5</v>
       </c>
       <c r="BU95">
-        <f>_xlfn.RANK.EQ(BS95,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>93</v>
       </c>
       <c r="BV95">
-        <f>_xlfn.RANK.EQ(AI95,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>48</v>
       </c>
       <c r="BW95" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX95" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -24535,27 +24535,27 @@
         <v>15</v>
       </c>
       <c r="BS96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="BT96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="BU96">
-        <f>_xlfn.RANK.EQ(BS96,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>93</v>
       </c>
       <c r="BV96">
-        <f>_xlfn.RANK.EQ(AI96,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>59</v>
       </c>
       <c r="BW96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX96" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>
@@ -24762,27 +24762,27 @@
         <v>2</v>
       </c>
       <c r="BS97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="BT97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5.99</v>
       </c>
       <c r="BU97">
-        <f>_xlfn.RANK.EQ(BS97,$BS$2:$BS$97)</f>
+        <f t="shared" si="13"/>
         <v>96</v>
       </c>
       <c r="BV97">
-        <f>_xlfn.RANK.EQ(AI97,$AI$2:$AI$97)</f>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="BW97" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>Bottom 5</v>
       </c>
       <c r="BX97" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>Bottom 5</v>
       </c>
     </row>

</xml_diff>